<commit_message>
UPDATE: the excel file, this file its an another backup to the data get in the salesforce database and callrail
</commit_message>
<xml_diff>
--- a/src/REPORT RADIO.VIVA.xlsx
+++ b/src/REPORT RADIO.VIVA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlbertoAlejandroMart\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C26D08D-3E52-472E-A26D-24AE76BFD78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFD99EB-AD67-4CC3-B678-00188D7ED6C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>CALLRAIL</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>BEFORE JULY</t>
+  </si>
+  <si>
+    <t>Its the 65-Cancelled Consult  not the Cancelled 90 days</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,6 +532,9 @@
       <c r="B10" s="1">
         <v>1</v>
       </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -618,6 +624,9 @@
       </c>
       <c r="B21" s="1">
         <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>